<commit_message>
Se cambia test tarjeta credito doble a long, y se termina el método
</commit_message>
<xml_diff>
--- a/docs/CasosPrueba - Validación/CP - NIF.xlsx
+++ b/docs/CasosPrueba - Validación/CP - NIF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adri_\source\repos\TDD-ACB-JGA\docs\CasosPrueba - Validación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8564AD-A408-4705-AF00-B7A0F244687E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABFEAE3-81AF-45C4-8D2E-52ACAD06D12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12BA3133-949C-4B91-9275-35525239132A}"/>
+    <workbookView xWindow="4365" yWindow="1350" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="3" xr2:uid="{12BA3133-949C-4B91-9275-35525239132A}"/>
   </bookViews>
   <sheets>
     <sheet name="CP-VAL-NIF-001" sheetId="1" r:id="rId1"/>
@@ -412,13 +412,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -440,15 +449,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1118,7 +1118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764A93F3-67DD-4594-9FAF-AC6E80869C56}">
   <dimension ref="B2:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -1132,10 +1132,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1147,10 +1147,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1160,10 +1160,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -1175,13 +1175,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
@@ -1207,73 +1207,73 @@
       <c r="F8" s="23"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1285,10 +1285,10 @@
       <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="7">
         <v>0</v>
       </c>
@@ -1300,10 +1300,10 @@
       <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7">
         <v>0</v>
       </c>
@@ -1315,8 +1315,8 @@
       <c r="B18" s="6">
         <v>3</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -1333,65 +1333,65 @@
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>2</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="17"/>
+      <c r="D24" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="13"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="4" t="s">
         <v>19</v>
       </c>
@@ -1402,13 +1402,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="B4:C4"/>
@@ -1425,6 +1418,13 @@
     <mergeCell ref="C20:F20"/>
     <mergeCell ref="B6:F8"/>
     <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <conditionalFormatting sqref="D26">
     <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
@@ -1459,10 +1459,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1474,10 +1474,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1487,10 +1487,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -1502,13 +1502,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
@@ -1534,35 +1534,35 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
@@ -1579,41 +1579,41 @@
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>4</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1625,10 +1625,10 @@
       <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7">
         <v>6</v>
       </c>
@@ -1640,8 +1640,8 @@
       <c r="B18" s="6">
         <v>2</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -1649,8 +1649,8 @@
       <c r="B19" s="6">
         <v>3</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
@@ -1667,65 +1667,65 @@
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>1</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
         <v>2</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="4" t="s">
         <v>19</v>
       </c>
@@ -1736,6 +1736,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="D25:F26"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1748,18 +1760,6 @@
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="D25:F26"/>
   </mergeCells>
   <conditionalFormatting sqref="D27">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
@@ -1794,10 +1794,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1809,10 +1809,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1822,10 +1822,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -1837,13 +1837,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
@@ -1869,35 +1869,35 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
@@ -1914,41 +1914,41 @@
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>4</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1960,10 +1960,10 @@
       <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7">
         <v>7</v>
       </c>
@@ -1975,8 +1975,8 @@
       <c r="B18" s="6">
         <v>2</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -1984,8 +1984,8 @@
       <c r="B19" s="6">
         <v>3</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
@@ -2002,65 +2002,65 @@
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>1</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
         <v>2</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="4" t="s">
         <v>19</v>
       </c>
@@ -2071,6 +2071,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="D25:F26"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -2083,18 +2095,6 @@
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="D25:F26"/>
   </mergeCells>
   <conditionalFormatting sqref="D27">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
@@ -2129,10 +2129,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2144,10 +2144,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -2157,10 +2157,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -2172,13 +2172,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
@@ -2204,73 +2204,73 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
@@ -2282,10 +2282,10 @@
       <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="7">
         <v>0</v>
       </c>
@@ -2297,8 +2297,8 @@
       <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
@@ -2306,8 +2306,8 @@
       <c r="B18" s="6">
         <v>3</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -2324,65 +2324,65 @@
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>2</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="17"/>
+      <c r="D24" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="13"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="4" t="s">
         <v>19</v>
       </c>
@@ -2393,12 +2393,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F8"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:F25"/>
+    <mergeCell ref="B26:C26"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C11:F11"/>
@@ -2411,11 +2410,12 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:F25"/>
-    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="D26">
     <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
@@ -2437,7 +2437,7 @@
   <dimension ref="B2:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B6" sqref="B6:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2450,10 +2450,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2465,10 +2465,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -2478,10 +2478,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -2493,13 +2493,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
@@ -2525,75 +2525,75 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
@@ -2605,10 +2605,10 @@
       <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="7">
         <v>0</v>
       </c>
@@ -2620,8 +2620,8 @@
       <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
@@ -2629,8 +2629,8 @@
       <c r="B18" s="6">
         <v>3</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -2647,65 +2647,65 @@
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>2</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="17"/>
+      <c r="D24" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="13"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="4" t="s">
         <v>19</v>
       </c>
@@ -2716,12 +2716,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F8"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:F25"/>
+    <mergeCell ref="B26:C26"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C11:F11"/>
@@ -2734,11 +2733,12 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:F25"/>
-    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="D26">
     <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
@@ -2759,8 +2759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810CD538-B272-4A79-BE86-D9E27E36EEB4}">
   <dimension ref="B2:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2773,10 +2773,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -2788,10 +2788,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -2801,10 +2801,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -2816,13 +2816,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
@@ -2848,35 +2848,35 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
@@ -2893,41 +2893,41 @@
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>4</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
@@ -2939,10 +2939,10 @@
       <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7">
         <v>0</v>
       </c>
@@ -2954,8 +2954,8 @@
       <c r="B18" s="6">
         <v>2</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -2963,8 +2963,8 @@
       <c r="B19" s="6">
         <v>3</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
@@ -2981,65 +2981,65 @@
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>1</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
         <v>2</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="4" t="s">
         <v>19</v>
       </c>
@@ -3050,12 +3050,11 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F8"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="D25:F26"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C11:F11"/>
@@ -3069,11 +3068,12 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="D25:F26"/>
-    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="D27">
     <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
@@ -3108,10 +3108,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -3123,10 +3123,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -3136,10 +3136,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -3151,13 +3151,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
@@ -3183,35 +3183,35 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
@@ -3228,41 +3228,41 @@
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>4</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
@@ -3274,10 +3274,10 @@
       <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7">
         <v>1</v>
       </c>
@@ -3289,8 +3289,8 @@
       <c r="B18" s="6">
         <v>2</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -3298,8 +3298,8 @@
       <c r="B19" s="6">
         <v>3</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
@@ -3316,65 +3316,65 @@
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>1</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
         <v>2</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="4" t="s">
         <v>19</v>
       </c>
@@ -3385,6 +3385,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="D25:F26"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -3397,18 +3409,6 @@
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="D25:F26"/>
   </mergeCells>
   <conditionalFormatting sqref="D27">
     <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
@@ -3443,10 +3443,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -3458,10 +3458,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -3471,10 +3471,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -3486,13 +3486,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
@@ -3518,35 +3518,35 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
@@ -3563,41 +3563,41 @@
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>4</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
@@ -3609,10 +3609,10 @@
       <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7">
         <v>2</v>
       </c>
@@ -3624,8 +3624,8 @@
       <c r="B18" s="6">
         <v>2</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -3633,8 +3633,8 @@
       <c r="B19" s="6">
         <v>3</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
@@ -3651,65 +3651,65 @@
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>1</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
         <v>2</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="4" t="s">
         <v>19</v>
       </c>
@@ -3720,6 +3720,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="D25:F26"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -3732,18 +3744,6 @@
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="D25:F26"/>
   </mergeCells>
   <conditionalFormatting sqref="D27">
     <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
@@ -3778,10 +3778,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -3793,10 +3793,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -3806,10 +3806,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -3821,13 +3821,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
@@ -3853,35 +3853,35 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
@@ -3898,41 +3898,41 @@
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>4</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
@@ -3944,10 +3944,10 @@
       <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7">
         <v>3</v>
       </c>
@@ -3959,8 +3959,8 @@
       <c r="B18" s="6">
         <v>2</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -3968,8 +3968,8 @@
       <c r="B19" s="6">
         <v>3</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
@@ -3986,65 +3986,65 @@
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>1</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
         <v>2</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="4" t="s">
         <v>19</v>
       </c>
@@ -4055,6 +4055,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="D25:F26"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -4067,18 +4079,6 @@
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="D25:F26"/>
   </mergeCells>
   <conditionalFormatting sqref="D27">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
@@ -4113,10 +4113,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -4128,10 +4128,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -4141,10 +4141,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -4156,13 +4156,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
@@ -4188,35 +4188,35 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
@@ -4233,41 +4233,41 @@
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>4</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
@@ -4279,10 +4279,10 @@
       <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7">
         <v>4</v>
       </c>
@@ -4294,8 +4294,8 @@
       <c r="B18" s="6">
         <v>2</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -4303,8 +4303,8 @@
       <c r="B19" s="6">
         <v>3</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
@@ -4321,65 +4321,65 @@
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>1</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
         <v>2</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="4" t="s">
         <v>19</v>
       </c>
@@ -4390,6 +4390,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="D25:F26"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -4402,18 +4414,6 @@
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="D25:F26"/>
   </mergeCells>
   <conditionalFormatting sqref="D27">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -4448,10 +4448,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -4463,10 +4463,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -4476,10 +4476,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -4491,13 +4491,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
@@ -4523,35 +4523,35 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
@@ -4568,41 +4568,41 @@
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>4</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="18"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
@@ -4614,10 +4614,10 @@
       <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7">
         <v>5</v>
       </c>
@@ -4629,8 +4629,8 @@
       <c r="B18" s="6">
         <v>2</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -4638,8 +4638,8 @@
       <c r="B19" s="6">
         <v>3</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
@@ -4656,65 +4656,65 @@
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>1</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
         <v>2</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="13"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="4" t="s">
         <v>19</v>
       </c>
@@ -4725,6 +4725,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="D25:F26"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -4737,18 +4749,6 @@
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="D25:F26"/>
   </mergeCells>
   <conditionalFormatting sqref="D27">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">

</xml_diff>